<commit_message>
Check if users data is stored correctly
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -784,12 +784,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Olga</t>
+          <t>Yana</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>olga@inbox.com</t>
+          <t>yana@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add banner, edit  text style and colors
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -784,12 +784,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Yana</t>
+          <t>Yha</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>yana@gmail.com</t>
+          <t>sfs@sdffs.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit text colors and add thank you banner to the end of test
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -784,12 +784,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Yha</t>
+          <t>sdsfd</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sfs@sdffs.com</t>
+          <t>sdfd@sdfds.ccc</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Insert user data to the worksheet
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,6 +34,13 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,10 +60,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -65,9 +76,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -436,7 +449,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="87" customWidth="1" min="1" max="1"/>
     <col width="11.85546875" customWidth="1" style="3" min="2" max="2"/>
@@ -574,7 +587,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="82" customWidth="1" min="1" max="1"/>
   </cols>
@@ -668,7 +681,7 @@
       <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="71" customWidth="1" min="1" max="1"/>
     <col width="12.42578125" customWidth="1" min="2" max="2"/>
@@ -752,21 +765,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35.5703125" customWidth="1" min="1" max="1"/>
+    <col width="31.85546875" customWidth="1" min="1" max="1"/>
     <col width="25.5703125" customWidth="1" min="2" max="2"/>
+    <col width="14.140625" customWidth="1" min="3" max="3"/>
+    <col width="11.5703125" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -780,20 +795,80 @@
           <t>E-mail</t>
         </is>
       </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sdsfd</t>
+          <t>dfs</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sdfd@sdfds.ccc</t>
+          <t>sdf@dfd.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>dggfh</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>sdf@sdf.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>intra</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fffff</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>sdff@sdfds.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>intra</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sahsa</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sasha@ddd.ccc</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uncomment code in function check_data
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -770,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -864,6 +864,42 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tanja</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tanja@fvv.ccc</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Olga</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>olga@gcm.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Olga</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>olga@tan.ccc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit function to clear terminal window
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -770,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -900,6 +900,18 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Irina</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>irina@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit function to clear window step 3
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -770,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -912,6 +912,30 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>usdf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sdf@sdf.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sdsdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sdfsd@sdf.ccc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit function to clear terminal window step 4
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -770,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -936,6 +936,18 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>iii</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sdfsd@dsfsd.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Check if user data is already in the worksheet
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,13 +34,6 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,14 +53,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -76,11 +65,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -765,15 +752,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -804,87 +791,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dfs</t>
+          <t>Olga</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sdf@dfd.com</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>extra</t>
+          <t>olga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dggfh</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>sdf@sdf.com</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>intra</t>
+          <t>Una</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>una@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>fffff</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>sdff@sdfds.com</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>intra</t>
+          <t>Tanja</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tanja@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sahsa</t>
+          <t>Olga</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sasha@ddd.ccc</t>
+          <t>olga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tanja</t>
+          <t>Olga</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>tanja@fvv.ccc</t>
+          <t>olga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Olga</t>
+          <t>Lena</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>olga@gcm.com</t>
+          <t>lena@gmail.com</t>
         </is>
       </c>
     </row>
@@ -896,99 +868,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>olga@tan.ccc</t>
+          <t>olga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Irina</t>
+          <t>Olga</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>irina@gmail.com</t>
+          <t>olga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>usdf</t>
+          <t>Lena</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sdf@sdf.com</t>
+          <t>lena@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sdsdf</t>
+          <t>Tanja</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sdfsd@sdf.ccc</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>iii</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>sdfsd@dsfsd.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>yyy</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>sdfd@dsfs.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>yyy</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ttt@ccc.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>yy</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>sdfsd@sdf.com</t>
+          <t>tanja@gmail.com</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reorganize code to call functions from main start_test function
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,17 +757,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31.85546875" customWidth="1" min="1" max="1"/>
     <col width="25.5703125" customWidth="1" min="2" max="2"/>
-    <col width="14.140625" customWidth="1" min="3" max="3"/>
+    <col width="14.140625" customWidth="1" style="3" min="3" max="3"/>
     <col width="11.5703125" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -908,6 +908,51 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Katja</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>katja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tanja</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>tanja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Julja</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>julja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add loop to check repeat user or new user
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,7 +757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -848,6 +848,36 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Yulja</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>yulja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tanja</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>tanja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Overwrite test result to worksheet cell of existing user
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -760,7 +760,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -833,51 +833,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Tanja</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>tanja@gmail.com</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Yulja</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>yulja@gmail.com</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>tanja</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>tanja@gmail.com</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-9</v>
-      </c>
-    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug with overwriting user information in the worksheet
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,10 +757,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4">
@@ -830,12 +830,24 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lena</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>lena@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bugs in writing user data to worksheet
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,7 +757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
@@ -848,6 +848,81 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rita</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>rita@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rita</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>rita@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sasha</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sasha@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>dasha</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>dasha@gnail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Nadja</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>nadja@gmail.com</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug of user data duplication in worksheet
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,10 +757,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A7" sqref="A7:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -860,69 +860,14 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Rita</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>rita@gmail.com</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sasha</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>sasha@gmail.com</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>dasha</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>dasha@gnail.com</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Nadja</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>nadja@gmail.com</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-    </row>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add and edit comments to functions
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -757,7 +757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD12"/>
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
@@ -863,11 +863,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Hanna</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>hanna@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize creating instances from workbook
</commit_message>
<xml_diff>
--- a/test_e_i.xlsx
+++ b/test_e_i.xlsx
@@ -760,7 +760,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6">

</xml_diff>